<commit_message>
number of libraries (for all mun)
new value-driven feature
</commit_message>
<xml_diff>
--- a/migforecasting/superdataset/superset features.xlsx
+++ b/migforecasting/superdataset/superset features.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="All features" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="94">
   <si>
     <t>категория</t>
   </si>
@@ -293,6 +293,15 @@
   </si>
   <si>
     <t>docsnum</t>
+  </si>
+  <si>
+    <t>NEW (value-driven)</t>
+  </si>
+  <si>
+    <t>Число библиотек - library (шт.) (8017001)</t>
+  </si>
+  <si>
+    <t>library</t>
   </si>
 </sst>
 </file>
@@ -401,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -432,6 +441,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -714,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J33"/>
+  <dimension ref="B2:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,8 +1361,37 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="7"/>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G33" s="7">
+        <v>31</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I33" s="5">
+        <v>195097</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1362,7 +1403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
cultureorg for all mun (value-driven feature)
</commit_message>
<xml_diff>
--- a/migforecasting/superdataset/superset features.xlsx
+++ b/migforecasting/superdataset/superset features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="96">
   <si>
     <t>категория</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Доходы бюд. - budincome (тыс. руб) (8013001)</t>
   </si>
   <si>
-    <t>Развлечения (счастье?)</t>
-  </si>
-  <si>
     <t>Число музеев - museums (шт.) (8017004)</t>
   </si>
   <si>
@@ -302,6 +299,15 @@
   </si>
   <si>
     <t>library</t>
+  </si>
+  <si>
+    <t>Орг. культ-досуг типа - cultureorg (шт.) (8016001)</t>
+  </si>
+  <si>
+    <t>cultureorg</t>
+  </si>
+  <si>
+    <t>Развлечения (счастье?) (value-driven)</t>
   </si>
 </sst>
 </file>
@@ -410,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -426,9 +432,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -726,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J35"/>
+  <dimension ref="B2:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,16 +749,16 @@
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G2" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
@@ -774,14 +777,14 @@
       <c r="G3" s="5">
         <v>1</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>42</v>
+      <c r="H3" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="I3" s="5">
         <v>227872</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
@@ -801,14 +804,14 @@
         <f>1+G3</f>
         <v>2</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>43</v>
+      <c r="H4" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="I4" s="5">
         <v>212760</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -823,17 +826,17 @@
         <v>13</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" ref="G5:G32" si="0">1+G4</f>
+        <f t="shared" ref="G5:G35" si="0">1+G4</f>
         <v>3</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="8">
+      <c r="H5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="7">
         <v>37560</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>84</v>
+      <c r="J5" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -844,14 +847,14 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="8">
+      <c r="H6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="7">
         <v>37259</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>84</v>
+      <c r="J6" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -862,14 +865,14 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>46</v>
+      <c r="H7" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="I7" s="5">
         <v>293422</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -877,14 +880,14 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>47</v>
+      <c r="H8" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="I8" s="5">
         <v>133378</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -892,14 +895,14 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>48</v>
+      <c r="H9" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="I9" s="5">
         <v>29890</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -919,14 +922,14 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>49</v>
+      <c r="H10" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="I10" s="5">
         <v>19826</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -946,14 +949,14 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H11" s="9" t="s">
-        <v>50</v>
+      <c r="H11" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="I11" s="5">
         <v>236577</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -971,14 +974,14 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>51</v>
+      <c r="H12" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="I12" s="5">
         <v>8270</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -992,14 +995,14 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="H13" s="9" t="s">
-        <v>52</v>
+      <c r="H13" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="I13" s="5">
         <v>36115</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -1010,14 +1013,14 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>53</v>
+      <c r="H14" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="I14" s="5">
         <v>349314</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
@@ -1025,14 +1028,14 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="H15" s="9" t="s">
-        <v>54</v>
+      <c r="H15" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="I15" s="5">
         <v>150541</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
@@ -1040,14 +1043,14 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H16" s="9" t="s">
-        <v>55</v>
+      <c r="H16" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="I16" s="5">
         <v>202665</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -1058,23 +1061,23 @@
         <v>26</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G17" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H17" s="9" t="s">
-        <v>56</v>
+      <c r="H17" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="I17" s="5">
         <v>33934</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -1085,23 +1088,23 @@
         <v>25</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G18" s="5">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="H18" s="9" t="s">
-        <v>57</v>
+      <c r="H18" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="I18" s="5">
         <v>33234</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -1110,47 +1113,47 @@
         <v>27</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G19" s="5">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>58</v>
+      <c r="H19" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="I19" s="5">
         <v>32697</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G20" s="5">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H20" s="9" t="s">
-        <v>59</v>
+      <c r="H20" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="I20" s="5">
         <v>104267</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -1158,14 +1161,14 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="H21" s="9" t="s">
-        <v>60</v>
+      <c r="H21" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="I21" s="5">
         <v>312731</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -1173,14 +1176,14 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H22" s="9" t="s">
-        <v>61</v>
+      <c r="H22" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="I22" s="5">
         <v>128832</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -1188,14 +1191,14 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="H23" s="9" t="s">
-        <v>62</v>
+      <c r="H23" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="I23" s="5">
         <v>40224</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1203,14 +1206,14 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="H24" s="9" t="s">
-        <v>63</v>
+      <c r="H24" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="I24" s="5">
         <v>15759</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -1218,14 +1221,14 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="H25" s="9" t="s">
-        <v>64</v>
+      <c r="H25" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="I25" s="5">
         <v>9458</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
@@ -1233,14 +1236,14 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="H26" s="9" t="s">
-        <v>65</v>
+      <c r="H26" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="I26" s="5">
         <v>180489</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
@@ -1248,26 +1251,26 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G27" s="5">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="H27" s="9" t="s">
-        <v>66</v>
+      <c r="H27" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="I27" s="5">
         <v>61414</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
@@ -1275,45 +1278,45 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G28" s="5">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="H28" s="11" t="s">
-        <v>90</v>
+      <c r="H28" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="I28" s="5">
         <v>61956</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="C29" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G29" s="5">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="H29" s="9" t="s">
-        <v>67</v>
+      <c r="H29" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="I29" s="5">
         <v>96237</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
@@ -1321,14 +1324,14 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="H30" s="9" t="s">
-        <v>68</v>
+      <c r="H30" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="I30" s="5">
         <v>248264</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
@@ -1336,14 +1339,14 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="H31" s="9" t="s">
-        <v>69</v>
+      <c r="H31" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="I31" s="5">
         <v>39682</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
@@ -1351,14 +1354,14 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H32" s="10" t="s">
-        <v>86</v>
+      <c r="H32" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="I32" s="5">
         <v>23486</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
@@ -1366,19 +1369,20 @@
         <v>0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G33" s="7">
+        <v>90</v>
+      </c>
+      <c r="G33" s="5">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="H33" s="12" t="s">
-        <v>93</v>
+      <c r="H33" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="I33" s="5">
         <v>195097</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
@@ -1386,12 +1390,34 @@
         <v>3</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="G34" s="5">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I34" s="5">
+        <v>225133</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
-      <c r="C35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G35" s="5">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1416,30 +1442,30 @@
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>12</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>53</v>
+      <c r="C4" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="D4" s="5">
         <v>349314</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J4" s="5"/>
     </row>
@@ -1447,14 +1473,14 @@
       <c r="B5" s="5">
         <v>19</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>60</v>
+      <c r="C5" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="D5" s="5">
         <v>312731</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J5" s="5"/>
     </row>
@@ -1462,14 +1488,14 @@
       <c r="B6" s="5">
         <v>5</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>46</v>
+      <c r="C6" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="D6" s="5">
         <v>293422</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J6" s="5"/>
     </row>
@@ -1477,14 +1503,14 @@
       <c r="B7" s="5">
         <v>28</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>68</v>
+      <c r="C7" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="D7" s="5">
         <v>248264</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J7" s="5"/>
     </row>
@@ -1492,14 +1518,14 @@
       <c r="B8" s="5">
         <v>9</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>50</v>
+      <c r="C8" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="D8" s="5">
         <v>236577</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J8" s="5"/>
     </row>
@@ -1507,14 +1533,14 @@
       <c r="B9" s="5">
         <v>1</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>42</v>
+      <c r="C9" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="D9" s="5">
         <v>227872</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J9" s="5"/>
     </row>
@@ -1522,14 +1548,14 @@
       <c r="B10" s="5">
         <v>2</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>43</v>
+      <c r="C10" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="D10" s="5">
         <v>212760</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J10" s="5"/>
     </row>
@@ -1537,14 +1563,14 @@
       <c r="B11" s="5">
         <v>14</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>55</v>
+      <c r="C11" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="D11" s="5">
         <v>202665</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J11" s="5"/>
     </row>
@@ -1552,14 +1578,14 @@
       <c r="B12" s="5">
         <v>24</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>65</v>
+      <c r="C12" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="D12" s="5">
         <v>180489</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J12" s="5"/>
     </row>
@@ -1567,14 +1593,14 @@
       <c r="B13" s="5">
         <v>13</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>54</v>
+      <c r="C13" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="D13" s="5">
         <v>150541</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J13" s="5"/>
     </row>
@@ -1582,14 +1608,14 @@
       <c r="B14" s="5">
         <v>6</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>47</v>
+      <c r="C14" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="D14" s="5">
         <v>133378</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J14" s="5"/>
     </row>
@@ -1597,14 +1623,14 @@
       <c r="B15" s="5">
         <v>20</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>61</v>
+      <c r="C15" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="D15" s="5">
         <v>128832</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J15" s="5"/>
     </row>
@@ -1612,14 +1638,14 @@
       <c r="B16" s="5">
         <v>18</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>59</v>
+      <c r="C16" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="D16" s="5">
         <v>104267</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J16" s="5"/>
     </row>
@@ -1627,14 +1653,14 @@
       <c r="B17" s="5">
         <v>27</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>67</v>
+      <c r="C17" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="D17" s="5">
         <v>96237</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J17" s="5"/>
     </row>
@@ -1642,14 +1668,14 @@
       <c r="B18" s="5">
         <v>26</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>90</v>
+      <c r="C18" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="D18" s="5">
         <v>61956</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J18" s="5"/>
     </row>
@@ -1657,14 +1683,14 @@
       <c r="B19" s="5">
         <v>25</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>66</v>
+      <c r="C19" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="D19" s="5">
         <v>61414</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J19" s="5"/>
     </row>
@@ -1672,14 +1698,14 @@
       <c r="B20" s="5">
         <v>21</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>62</v>
+      <c r="C20" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="D20" s="5">
         <v>40224</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J20" s="5"/>
     </row>
@@ -1687,14 +1713,14 @@
       <c r="B21" s="5">
         <v>29</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>69</v>
+      <c r="C21" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="D21" s="5">
         <v>39682</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J21" s="5"/>
     </row>
@@ -1702,14 +1728,14 @@
       <c r="B22" s="5">
         <v>3</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="8">
+      <c r="C22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="7">
         <v>37560</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>84</v>
+      <c r="E22" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="J22" s="5"/>
     </row>
@@ -1717,14 +1743,14 @@
       <c r="B23" s="5">
         <v>4</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="8">
+      <c r="C23" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="7">
         <v>37259</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>84</v>
+      <c r="E23" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="J23" s="5"/>
     </row>
@@ -1732,14 +1758,14 @@
       <c r="B24" s="5">
         <v>11</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>52</v>
+      <c r="C24" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="D24" s="5">
         <v>36115</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J24" s="5"/>
     </row>
@@ -1747,14 +1773,14 @@
       <c r="B25" s="5">
         <v>15</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>56</v>
+      <c r="C25" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="D25" s="5">
         <v>33934</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J25" s="5"/>
     </row>
@@ -1762,14 +1788,14 @@
       <c r="B26" s="5">
         <v>16</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>57</v>
+      <c r="C26" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="D26" s="5">
         <v>33234</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J26" s="5"/>
     </row>
@@ -1777,14 +1803,14 @@
       <c r="B27" s="5">
         <v>17</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>58</v>
+      <c r="C27" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="D27" s="5">
         <v>32697</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J27" s="5"/>
     </row>
@@ -1792,14 +1818,14 @@
       <c r="B28" s="5">
         <v>7</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>48</v>
+      <c r="C28" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="D28" s="5">
         <v>29890</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J28" s="5"/>
     </row>
@@ -1807,14 +1833,14 @@
       <c r="B29" s="5">
         <v>30</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>86</v>
+      <c r="C29" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="D29" s="5">
         <v>23486</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J29" s="5"/>
     </row>
@@ -1822,14 +1848,14 @@
       <c r="B30" s="5">
         <v>8</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>49</v>
+      <c r="C30" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="D30" s="5">
         <v>19826</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J30" s="5"/>
     </row>
@@ -1837,14 +1863,14 @@
       <c r="B31" s="5">
         <v>22</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>63</v>
+      <c r="C31" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="D31" s="5">
         <v>15759</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J31" s="5"/>
     </row>
@@ -1852,14 +1878,14 @@
       <c r="B32" s="5">
         <v>23</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>64</v>
+      <c r="C32" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="D32" s="5">
         <v>9458</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J32" s="5"/>
     </row>
@@ -1867,14 +1893,14 @@
       <c r="B33" s="5">
         <v>10</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>51</v>
+      <c r="C33" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="D33" s="5">
         <v>8270</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
number of mus, art schools (for all mun)
</commit_message>
<xml_diff>
--- a/migforecasting/superdataset/superset features.xlsx
+++ b/migforecasting/superdataset/superset features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="99">
   <si>
     <t>категория</t>
   </si>
@@ -308,6 +308,15 @@
   </si>
   <si>
     <t>Развлечения (счастье?) (value-driven)</t>
+  </si>
+  <si>
+    <t>Число дет. муз, худ школ - musartschool (шт.) (8017010)</t>
+  </si>
+  <si>
+    <t>musartschool</t>
+  </si>
+  <si>
+    <t>2007 - 2017</t>
   </si>
 </sst>
 </file>
@@ -729,16 +738,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J36"/>
+  <dimension ref="B2:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" customWidth="1"/>
+    <col min="3" max="3" width="53.28515625" customWidth="1"/>
     <col min="4" max="4" width="58.140625" customWidth="1"/>
     <col min="5" max="5" width="62.28515625" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
@@ -1415,9 +1424,23 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
+      <c r="H35" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="I35" s="5">
+        <v>58942</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C36" s="2"/>
+      <c r="C36" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C37" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
superdataset-41 (with new value-driven features)
</commit_message>
<xml_diff>
--- a/migforecasting/superdataset/superset features.xlsx
+++ b/migforecasting/superdataset/superset features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="99">
   <si>
     <t>категория</t>
   </si>
@@ -425,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -456,6 +456,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -740,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,7 +1443,7 @@
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C37" s="2"/>
+      <c r="C37" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1450,10 +1453,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J33"/>
+  <dimension ref="B3:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,268 +1572,268 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
-        <v>2</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>42</v>
+        <v>32</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="D10" s="5">
-        <v>212760</v>
+        <v>225133</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D11" s="5">
-        <v>202665</v>
+        <v>212760</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D12" s="5">
-        <v>180489</v>
+        <v>202665</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
-        <v>13</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>53</v>
+        <v>31</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="D13" s="5">
-        <v>150541</v>
+        <v>195097</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D14" s="5">
-        <v>133378</v>
+        <v>180489</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D15" s="5">
-        <v>128832</v>
+        <v>150541</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D16" s="5">
-        <v>104267</v>
+        <v>133378</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D17" s="5">
-        <v>96237</v>
+        <v>128832</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
-        <v>26</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>89</v>
+        <v>18</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="D18" s="5">
-        <v>61956</v>
+        <v>104267</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D19" s="5">
-        <v>61414</v>
+        <v>96237</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="J19" s="5"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="5">
-        <v>21</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>61</v>
+        <v>26</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="D20" s="5">
-        <v>40224</v>
+        <v>61956</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="J20" s="5"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="5">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D21" s="5">
-        <v>39682</v>
+        <v>61414</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J21" s="5"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="5">
-        <v>3</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="7">
-        <v>37560</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>83</v>
+        <v>33</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="5">
+        <v>58942</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="J22" s="5"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="7">
-        <v>37259</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>83</v>
+        <v>61</v>
+      </c>
+      <c r="D23" s="5">
+        <v>40224</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="J23" s="5"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="5">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="D24" s="5">
-        <v>36115</v>
+        <v>39682</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="J24" s="5"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="5">
-        <v>33934</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>79</v>
+        <v>43</v>
+      </c>
+      <c r="D25" s="7">
+        <v>37560</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="J25" s="5"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="5">
-        <v>33234</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>79</v>
+        <v>44</v>
+      </c>
+      <c r="D26" s="7">
+        <v>37259</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="J26" s="5"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="5">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D27" s="5">
-        <v>32697</v>
+        <v>36115</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>79</v>
@@ -1839,96 +1842,138 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D28" s="5">
-        <v>29890</v>
+        <v>33934</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="J28" s="5"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="5">
-        <v>30</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>85</v>
+        <v>16</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="D29" s="5">
-        <v>23486</v>
+        <v>33234</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J29" s="5"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="5">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D30" s="5">
-        <v>19826</v>
+        <v>32697</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J30" s="5"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="5">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="D31" s="5">
-        <v>15759</v>
+        <v>29890</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="J31" s="5"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="5">
-        <v>23</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>63</v>
+        <v>30</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="D32" s="5">
-        <v>9458</v>
+        <v>23486</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="J32" s="5"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="5">
+        <v>8</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="5">
+        <v>19826</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="5">
+        <v>22</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="5">
+        <v>15759</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="5">
+        <v>23</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="5">
+        <v>9458</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="5">
         <v>10</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C36" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D36" s="5">
         <v>8270</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E36" s="5" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B4:E33">
-    <sortCondition descending="1" ref="D4:D33"/>
+  <sortState ref="B4:E36">
+    <sortCondition descending="1" ref="D4:D36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new feature - badcompanies
</commit_message>
<xml_diff>
--- a/migforecasting/superdataset/superset features.xlsx
+++ b/migforecasting/superdataset/superset features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="104">
   <si>
     <t>категория</t>
   </si>
@@ -326,6 +326,12 @@
   </si>
   <si>
     <t>goodcompanies</t>
+  </si>
+  <si>
+    <t>Кол-во убыточных орг. - badcompanies (шт.) (8042011)</t>
+  </si>
+  <si>
+    <t>badcompanies</t>
   </si>
 </sst>
 </file>
@@ -753,7 +759,7 @@
   <dimension ref="B2:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,7 +853,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" ref="G5:G35" si="0">1+G4</f>
+        <f t="shared" ref="G5:G37" si="0">1+G4</f>
         <v>3</v>
       </c>
       <c r="H5" s="8" t="s">
@@ -1438,6 +1444,9 @@
       <c r="C35" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="D35" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="G35" s="5">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1457,6 +1466,7 @@
         <v>96</v>
       </c>
       <c r="G36" s="5">
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="H36" s="11" t="s">
@@ -1471,6 +1481,19 @@
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C37" s="12"/>
+      <c r="G37" s="5">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="I37" s="5">
+        <v>39758</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new feature - visiblecompanies
</commit_message>
<xml_diff>
--- a/migforecasting/superdataset/superset features.xlsx
+++ b/migforecasting/superdataset/superset features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="106">
   <si>
     <t>категория</t>
   </si>
@@ -332,6 +332,12 @@
   </si>
   <si>
     <t>badcompanies</t>
+  </si>
+  <si>
+    <t>Кол-во орг. подав. отч. - visiblecompanies (шт.) (8042010)</t>
+  </si>
+  <si>
+    <t>visiblecompanies</t>
   </si>
 </sst>
 </file>
@@ -756,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J37"/>
+  <dimension ref="B2:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,7 +859,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" ref="G5:G37" si="0">1+G4</f>
+        <f t="shared" ref="G5:G38" si="0">1+G4</f>
         <v>3</v>
       </c>
       <c r="H5" s="8" t="s">
@@ -1465,6 +1471,9 @@
       <c r="C36" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="D36" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="G36" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1492,6 +1501,21 @@
         <v>39758</v>
       </c>
       <c r="J37" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G38" s="5">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I38" s="5">
+        <v>63004</v>
+      </c>
+      <c r="J38" s="5" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new feature - goodcompincome
</commit_message>
<xml_diff>
--- a/migforecasting/superdataset/superset features.xlsx
+++ b/migforecasting/superdataset/superset features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="108">
   <si>
     <t>категория</t>
   </si>
@@ -338,6 +338,12 @@
   </si>
   <si>
     <t>visiblecompanies</t>
+  </si>
+  <si>
+    <t>Фин. результат. приб. орг. - goodcompincome (тыс. руб.) (8042016)</t>
+  </si>
+  <si>
+    <t>goodcompincome</t>
   </si>
 </sst>
 </file>
@@ -762,17 +768,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J38"/>
+  <dimension ref="B2:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="53.28515625" customWidth="1"/>
-    <col min="4" max="4" width="58.140625" customWidth="1"/>
+    <col min="4" max="4" width="62.5703125" customWidth="1"/>
     <col min="5" max="5" width="62.28515625" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
     <col min="8" max="8" width="19.140625" customWidth="1"/>
@@ -859,7 +865,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" ref="G5:G38" si="0">1+G4</f>
+        <f t="shared" ref="G5:G39" si="0">1+G4</f>
         <v>3</v>
       </c>
       <c r="H5" s="8" t="s">
@@ -1490,6 +1496,9 @@
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C37" s="12"/>
+      <c r="D37" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="G37" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1516,6 +1525,21 @@
         <v>63004</v>
       </c>
       <c r="J38" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G39" s="5">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I39" s="5">
+        <v>50315</v>
+      </c>
+      <c r="J39" s="5" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>